<commit_message>
projet terminé, validé au W3C 5html et css), à voir quelques détails
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
   <si>
     <t>Catégorie</t>
   </si>
@@ -47,93 +47,680 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>(SEO ou accessiblité ?)</t>
-  </si>
-  <si>
-    <t>langue mise sur "Default"</t>
-  </si>
-  <si>
-    <t>Titre absent</t>
-  </si>
-  <si>
-    <t>Description vide</t>
-  </si>
-  <si>
-    <t>Manque balise meta robots</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
-    <t>keywords + nom marque</t>
-  </si>
-  <si>
-    <t>balise meta keywords inutile</t>
-  </si>
-  <si>
-    <t>Elle est inutile car Google ne la prend pas en compte pour le référencement</t>
-  </si>
-  <si>
-    <t>balise défault pour personnes ne parlant aucune des langues si jamais le site est multilangue</t>
-  </si>
-  <si>
-    <t>ça améliore la crawbilité pour une meilleur indexation, Cela indique aux moteurs de recherche qu'ils doivent indexer la page (index) et suivre les liens présents sur celle-ci (follow)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ces balises indiquent aux moteurs de recherche de quoi traite la page. Elles sont aussi affichées dans les résultats. Elles doivent donc non seulement contenir le mot-clé visé, mais aussi donner envie au visiteur de cliquer pour lire notre page.
-</t>
-  </si>
-  <si>
-    <t>lien non de qualité</t>
-  </si>
-  <si>
-    <t>aucune cohérence avec notre coeur de métier + footer inutile (aucune force) + spam</t>
-  </si>
-  <si>
-    <t>les 2 balises keywords</t>
-  </si>
-  <si>
-    <t>black hat</t>
-  </si>
-  <si>
-    <t>structure des balises h</t>
-  </si>
-  <si>
-    <t>image moins lourde</t>
-  </si>
-  <si>
-    <t>logo à compresser</t>
-  </si>
-  <si>
-    <t>lien sur même page + lien déjà présent pour contact</t>
-  </si>
-  <si>
-    <t>hierarchie non respectée</t>
-  </si>
-  <si>
-    <t>cartographier la page avec des balises main, header, etc…</t>
-  </si>
-  <si>
-    <t>bouton contact pas assez de contraste</t>
-  </si>
-  <si>
-    <t>mettre texte plus foncé</t>
-  </si>
-  <si>
-    <t>augmenter taille texte et titre + gras</t>
-  </si>
-  <si>
-    <t>citation: alt n'est pas bon, spam et répétition</t>
-  </si>
-  <si>
-    <t>mettre la description de quoi il s'agit</t>
+    <t>lien des images ne sont pas vers les réseaux mais vers la page</t>
+  </si>
+  <si>
+    <t>ajout du titre pour accessibilité</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Balise importante pour que les outils d’accessibilité comme les lecteurs d’écrans puissent correctement prononcer les mots</t>
+  </si>
+  <si>
+    <r>
+      <t>Pas de titre dans la balise "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Toujours mettre la langue du site dans cette balise. Mettre "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" uniquement si le site est multilangues</t>
+    </r>
+  </si>
+  <si>
+    <t>Remplacer le "." par "La chouette agence - Entreprise web design Lyon"</t>
+  </si>
+  <si>
+    <t>Ajouter le nom de l'entreprise puis mots-clés comme titre</t>
+  </si>
+  <si>
+    <r>
+      <t>Ajouter "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>FR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" à la balise</t>
+    </r>
+  </si>
+  <si>
+    <t>Avoir une courte description de la page dans cette balise</t>
+  </si>
+  <si>
+    <t>Ecrire une présentation de la page dans cette balise en y incorporant les mots-clés</t>
+  </si>
+  <si>
+    <t>La description n'étant pas de haute qualité, cela rend notre page non pertinente et n'augmentera pas notre trafic de recherche</t>
+  </si>
+  <si>
+    <t>Cette balises indique aux moteurs de recherche de quoi traite la page. Cela doit montrer en quoi celui-ci répond à la requête saisie par l'internaute.</t>
+  </si>
+  <si>
+    <r>
+      <t>Pas de desription dans la balise meta "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Balise html "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>lang</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" mise sur "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Manque la balise meta "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>robots</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/debutants/balise-title</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-balise-meta-description/</t>
+  </si>
+  <si>
+    <r>
+      <t>Mettre un balise meta "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>robots</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" avec le lien "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>follow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>", cela indique aux moteurs de recherche qu'ils doivent indexer la page (index) et suivre les liens présents sur celle-ci (follow)</t>
+    </r>
+  </si>
+  <si>
+    <t>Crawbilité non améliorée pour une meilleur indexation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ajouter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&lt;meta name="robots" content="index, follow"&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">dans la balise </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;head&gt;&lt;/head&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>http://robots-txt.com/meta-robots/</t>
+  </si>
+  <si>
+    <r>
+      <t>balise meta "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>" est présente</t>
+    </r>
+  </si>
+  <si>
+    <t>Balise inutile pour le référencement</t>
+  </si>
+  <si>
+    <t>Ne pas mettre cette balise</t>
+  </si>
+  <si>
+    <t>La supprimer du code</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
+  </si>
+  <si>
+    <t>Mauvais pour le référencement, Google est plus à même de comprendre la page si les balises sont claires</t>
+  </si>
+  <si>
+    <t>Toujours utiliser ces balises pour montrer à Google les points importants</t>
+  </si>
+  <si>
+    <t>Les rajouter</t>
+  </si>
+  <si>
+    <t>https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/</t>
+  </si>
+  <si>
+    <r>
+      <t>Manque les balises sémantiques comme "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>header</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>footer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>", etc…</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Balises "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" inutiles et pratiquant le black hat</t>
+    </r>
+  </si>
+  <si>
+    <t>Ne jamais utiliser cette pratique, toujours insérer les mots-clés de façon naturelle dans du texte ou titres cohérents</t>
+  </si>
+  <si>
+    <t>Supprimer ces balises</t>
+  </si>
+  <si>
+    <t>https://fr.semrush.com/blog/seo-black-hat/</t>
+  </si>
+  <si>
+    <t>Lien sur la page où l'on est, et répétitions de liens vers une même page</t>
+  </si>
+  <si>
+    <t>multiplier les liens vers une même page en variant les ancres est une technique inutile en SEO car elle ne permet pas de positionner notre site sur plusieurs mots-clés.</t>
+  </si>
+  <si>
+    <t>Varier les supports sur lesquels nos liens sont positionnés (exemple image + texte), ou supprimer les liens en trop</t>
+  </si>
+  <si>
+    <t>Supprimer les répétitions des liens</t>
+  </si>
+  <si>
+    <t>https://www.joptimisemonsite.fr/astuce-seo-liens-identiques-meme-page/</t>
+  </si>
+  <si>
+    <t>Très mauvaise pratique de mettre les mots-clés de la même couleur que le fond (invisible pour l'utilisateur mais pas pour Google). Cela pénalise le référencement</t>
+  </si>
+  <si>
+    <t>Images trop lourdes</t>
+  </si>
+  <si>
+    <t>Images sans images mais avec du texte</t>
+  </si>
+  <si>
+    <t>Elles sont inutiles parce que le contenu peut être écrit entre des balises h ou p. Les images servent à illustrer du contenu et alourdissent la page.</t>
+  </si>
+  <si>
+    <t>Supprimer les images de texte et les remplacer par des balises avec du texte à l’intérieur.</t>
+  </si>
+  <si>
+    <t>N’utiliser des images que lorsque c’est nécessaire.</t>
+  </si>
+  <si>
+    <t>https://imageseo.io/images-seo-optimization/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" des images sont des spams, ne décrivent pas l'image</t>
+    </r>
+  </si>
+  <si>
+    <t>Le format des images n’est pas optimisé ce qui ralentit la vitesse du site</t>
+  </si>
+  <si>
+    <t>Favoriser des formats rapide à charger, et toujours dans des dimensions équivalentes à leur div</t>
+  </si>
+  <si>
+    <t>Compresser et changer les images</t>
+  </si>
+  <si>
+    <t>Pas de description de l'image, Google ne va pas comprendre le contenu de nos images + spam</t>
+  </si>
+  <si>
+    <r>
+      <t>Toujours mettre une description de l'image dans l'attribut "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Mettre une description de l'image</t>
+  </si>
+  <si>
+    <t>Pas assez de contraste sur le bouton "contact" et certains textes par rapport au background</t>
+  </si>
+  <si>
+    <t>Contraste insuffisant et ne permet pas une très bonne visibilité</t>
+  </si>
+  <si>
+    <t>Pour la conformité au niveau AA, le critère de succès WCAG 2.0 1.4.3 recommande que le texte normal ait un rapport de contraste minimum de 4,5:1 et que le texte de grande taille (18 points ou 14 points en gras) ait un rapport de contraste minimum de 3:1</t>
+  </si>
+  <si>
+    <t>Changer la couleur des textes pour avoir un bon ratio de contraste</t>
+  </si>
+  <si>
+    <t>https://dequeuniversity.com/tips/color-contrast</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Balises sémantiques </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> mal structuré</t>
+    </r>
+  </si>
+  <si>
+    <t>Les balises n'ont pas d'ordre hiérarchique</t>
+  </si>
+  <si>
+    <t>Utiliser qu'une seule balise H1, et ensuite les autres balises qui suivent doivent toujours être hierarchisées</t>
+  </si>
+  <si>
+    <t>Changer les hn pour tout hiérarchiser correctement</t>
+  </si>
+  <si>
+    <t>https://rank-it.fr/les-balises-hn/</t>
+  </si>
+  <si>
+    <t>La typographie peut être non visible car trop petite</t>
+  </si>
+  <si>
+    <t>Typographie trop petite</t>
+  </si>
+  <si>
+    <t>Toujours avoir un contenu lisible dès le départ</t>
+  </si>
+  <si>
+    <t>Changer la taille de la police ainsi que le "font-weight" si besoin</t>
+  </si>
+  <si>
+    <t>http://www.pompage.net/traduction/ameliorer-l-accessibilite-par-la-typographie</t>
+  </si>
+  <si>
+    <t>Liens dans le footer</t>
+  </si>
+  <si>
+    <t>Ils n'ont aucun intérêt et aucun rapport avec notre activité</t>
+  </si>
+  <si>
+    <t>Il faut avoir un annuaire dédié ou idéalement mettre les liens relatifs aux contenu dans une balise ancre</t>
+  </si>
+  <si>
+    <t>Supprimer tous les liens du footer</t>
+  </si>
+  <si>
+    <t>https://www.leptidigital.fr/webmarketing/seo/liens-footer-header-sitewide-6974/</t>
+  </si>
+  <si>
+    <t>Mieux espacé les questions et mettre des exemples</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6940878-decouvrez-les-exigences-en-matiere-daccessibilite</t>
+  </si>
+  <si>
+    <t>Formulaire pas clair, manque liaison label avec texte</t>
+  </si>
+  <si>
+    <r>
+      <t>Formulaire non espacé et pas d'instructions claires, manque l'attribut "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" à "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fournir de l'aide pour les formulaires + rajouter l'attribut "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" ayant la même valeur que l'id du champ</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,18 +742,32 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FFFFC000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -201,23 +802,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,17 +1061,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1045"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.29296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="4" width="21.29296875" customWidth="1"/>
-    <col min="5" max="5" width="18.703125" customWidth="1"/>
-    <col min="6" max="6" width="21.29296875" customWidth="1"/>
+    <col min="1" max="1" width="21.29296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="52.5546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="60.73828125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="57.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="74.2578125" style="4" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -449,19 +1082,19 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2"/>
@@ -485,189 +1118,365 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="5" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="7" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="9" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="11" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="16" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="20" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="22" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="24" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="28" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="30" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="32" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="37" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="39" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="42" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="4"/>
+      <c r="E45" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1634,8 +2443,43 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1026" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1027" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1028" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1029" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1030" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1031" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1032" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1033" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1034" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1035" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1036" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1037" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1038" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1039" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1040" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1041" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1042" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1043" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1044" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1045" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F7" r:id="rId3"/>
+    <hyperlink ref="F11" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remise en forme du logo
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
   <si>
     <t>Catégorie</t>
   </si>
@@ -50,12 +50,6 @@
     <t>SEO</t>
   </si>
   <si>
-    <t>lien des images ne sont pas vers les réseaux mais vers la page</t>
-  </si>
-  <si>
-    <t>ajout du titre pour accessibilité</t>
-  </si>
-  <si>
     <t>Accessibilité</t>
   </si>
   <si>
@@ -114,6 +108,582 @@
     <t>Ajouter le nom de l'entreprise puis mots-clés comme titre</t>
   </si>
   <si>
+    <t>Avoir une courte description de la page dans cette balise</t>
+  </si>
+  <si>
+    <t>Ecrire une présentation de la page dans cette balise en y incorporant les mots-clés</t>
+  </si>
+  <si>
+    <t>La description n'étant pas de haute qualité, cela rend notre page non pertinente et n'augmentera pas notre trafic de recherche</t>
+  </si>
+  <si>
+    <t>Cette balises indique aux moteurs de recherche de quoi traite la page. Cela doit montrer en quoi celui-ci répond à la requête saisie par l'internaute.</t>
+  </si>
+  <si>
+    <r>
+      <t>Pas de desription dans la balise meta "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Balise html "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>lang</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" mise sur "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Manque la balise meta "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>robots</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/debutants/balise-title</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-balise-meta-description/</t>
+  </si>
+  <si>
+    <r>
+      <t>Mettre un balise meta "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>robots</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" avec le lien "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>follow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>", cela indique aux moteurs de recherche qu'ils doivent indexer la page (index) et suivre les liens présents sur celle-ci (follow)</t>
+    </r>
+  </si>
+  <si>
+    <t>Crawbilité non améliorée pour une meilleur indexation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ajouter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&lt;meta name="robots" content="index, follow"&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">dans la balise </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;head&gt;&lt;/head&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>http://robots-txt.com/meta-robots/</t>
+  </si>
+  <si>
+    <r>
+      <t>balise meta "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>" est présente</t>
+    </r>
+  </si>
+  <si>
+    <t>Balise inutile pour le référencement</t>
+  </si>
+  <si>
+    <t>Ne pas mettre cette balise</t>
+  </si>
+  <si>
+    <t>La supprimer du code</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
+  </si>
+  <si>
+    <t>Mauvais pour le référencement, Google est plus à même de comprendre la page si les balises sont claires</t>
+  </si>
+  <si>
+    <t>Toujours utiliser ces balises pour montrer à Google les points importants</t>
+  </si>
+  <si>
+    <t>Les rajouter</t>
+  </si>
+  <si>
+    <t>https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/</t>
+  </si>
+  <si>
+    <r>
+      <t>Manque les balises sémantiques comme "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>header</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>footer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>", etc…</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Balises "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>keywords</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" inutiles et pratiquant le black hat</t>
+    </r>
+  </si>
+  <si>
+    <t>Ne jamais utiliser cette pratique, toujours insérer les mots-clés de façon naturelle dans du texte ou titres cohérents</t>
+  </si>
+  <si>
+    <t>Supprimer ces balises</t>
+  </si>
+  <si>
+    <t>https://fr.semrush.com/blog/seo-black-hat/</t>
+  </si>
+  <si>
+    <t>Lien sur la page où l'on est, et répétitions de liens vers une même page</t>
+  </si>
+  <si>
+    <t>multiplier les liens vers une même page en variant les ancres est une technique inutile en SEO car elle ne permet pas de positionner notre site sur plusieurs mots-clés.</t>
+  </si>
+  <si>
+    <t>Varier les supports sur lesquels nos liens sont positionnés (exemple image + texte), ou supprimer les liens en trop</t>
+  </si>
+  <si>
+    <t>Supprimer les répétitions des liens</t>
+  </si>
+  <si>
+    <t>https://www.joptimisemonsite.fr/astuce-seo-liens-identiques-meme-page/</t>
+  </si>
+  <si>
+    <t>Très mauvaise pratique de mettre les mots-clés de la même couleur que le fond (invisible pour l'utilisateur mais pas pour Google). Cela pénalise le référencement</t>
+  </si>
+  <si>
+    <t>Images trop lourdes</t>
+  </si>
+  <si>
+    <t>Images sans images mais avec du texte</t>
+  </si>
+  <si>
+    <t>Elles sont inutiles parce que le contenu peut être écrit entre des balises h ou p. Les images servent à illustrer du contenu et alourdissent la page.</t>
+  </si>
+  <si>
+    <t>Supprimer les images de texte et les remplacer par des balises avec du texte à l’intérieur.</t>
+  </si>
+  <si>
+    <t>N’utiliser des images que lorsque c’est nécessaire.</t>
+  </si>
+  <si>
+    <t>https://imageseo.io/images-seo-optimization/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" des images sont des spams, ne décrivent pas l'image</t>
+    </r>
+  </si>
+  <si>
+    <t>Le format des images n’est pas optimisé ce qui ralentit la vitesse du site</t>
+  </si>
+  <si>
+    <t>Favoriser des formats rapide à charger, et toujours dans des dimensions équivalentes à leur div</t>
+  </si>
+  <si>
+    <t>Compresser et changer les images</t>
+  </si>
+  <si>
+    <t>Pas de description de l'image, Google ne va pas comprendre le contenu de nos images + spam</t>
+  </si>
+  <si>
+    <r>
+      <t>Toujours mettre une description de l'image dans l'attribut "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Mettre une description de l'image</t>
+  </si>
+  <si>
+    <t>Pas assez de contraste sur le bouton "contact" et certains textes par rapport au background</t>
+  </si>
+  <si>
+    <t>Contraste insuffisant et ne permet pas une très bonne visibilité</t>
+  </si>
+  <si>
+    <t>Pour la conformité au niveau AA, le critère de succès WCAG 2.0 1.4.3 recommande que le texte normal ait un rapport de contraste minimum de 4,5:1 et que le texte de grande taille (18 points ou 14 points en gras) ait un rapport de contraste minimum de 3:1</t>
+  </si>
+  <si>
+    <t>Changer la couleur des textes pour avoir un bon ratio de contraste</t>
+  </si>
+  <si>
+    <t>https://dequeuniversity.com/tips/color-contrast</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Balises sémantiques </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> mal structuré</t>
+    </r>
+  </si>
+  <si>
+    <t>Les balises n'ont pas d'ordre hiérarchique</t>
+  </si>
+  <si>
+    <t>Utiliser qu'une seule balise H1, et ensuite les autres balises qui suivent doivent toujours être hierarchisées</t>
+  </si>
+  <si>
+    <t>Changer les hn pour tout hiérarchiser correctement</t>
+  </si>
+  <si>
+    <t>https://rank-it.fr/les-balises-hn/</t>
+  </si>
+  <si>
+    <t>La typographie peut être non visible car trop petite</t>
+  </si>
+  <si>
+    <t>Typographie trop petite</t>
+  </si>
+  <si>
+    <t>Toujours avoir un contenu lisible dès le départ</t>
+  </si>
+  <si>
+    <t>Changer la taille de la police ainsi que le "font-weight" si besoin</t>
+  </si>
+  <si>
+    <t>http://www.pompage.net/traduction/ameliorer-l-accessibilite-par-la-typographie</t>
+  </si>
+  <si>
+    <t>Liens dans le footer</t>
+  </si>
+  <si>
+    <t>Ils n'ont aucun intérêt et aucun rapport avec notre activité</t>
+  </si>
+  <si>
+    <t>Il faut avoir un annuaire dédié ou idéalement mettre les liens relatifs aux contenu dans une balise ancre</t>
+  </si>
+  <si>
+    <t>Supprimer tous les liens du footer</t>
+  </si>
+  <si>
+    <t>https://www.leptidigital.fr/webmarketing/seo/liens-footer-header-sitewide-6974/</t>
+  </si>
+  <si>
+    <t>Mieux espacé les questions et mettre des exemples</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6940878-decouvrez-les-exigences-en-matiere-daccessibilite</t>
+  </si>
+  <si>
+    <t>Formulaire pas clair, manque liaison label avec texte</t>
+  </si>
+  <si>
+    <r>
+      <t>Formulaire non espacé et pas d'instructions claires, manque l'attribut "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" à "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fournir de l'aide pour les formulaires + rajouter l'attribut "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" ayant la même valeur que l'id du champ</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>Ajouter "</t>
     </r>
@@ -124,7 +694,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>FR</t>
+      <t>fr</t>
     </r>
     <r>
       <rPr>
@@ -134,582 +704,6 @@
         <family val="2"/>
       </rPr>
       <t>" à la balise</t>
-    </r>
-  </si>
-  <si>
-    <t>Avoir une courte description de la page dans cette balise</t>
-  </si>
-  <si>
-    <t>Ecrire une présentation de la page dans cette balise en y incorporant les mots-clés</t>
-  </si>
-  <si>
-    <t>La description n'étant pas de haute qualité, cela rend notre page non pertinente et n'augmentera pas notre trafic de recherche</t>
-  </si>
-  <si>
-    <t>Cette balises indique aux moteurs de recherche de quoi traite la page. Cela doit montrer en quoi celui-ci répond à la requête saisie par l'internaute.</t>
-  </si>
-  <si>
-    <r>
-      <t>Pas de desription dans la balise meta "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>description</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Balise html "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>lang</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>" mise sur "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>default</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Manque la balise meta "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>robots</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <t>https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
-  </si>
-  <si>
-    <t>https://www.webrankinfo.com/dossiers/debutants/balise-title</t>
-  </si>
-  <si>
-    <t>https://smartkeyword.io/seo-on-page-balise-meta-description/</t>
-  </si>
-  <si>
-    <r>
-      <t>Mettre un balise meta "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>robots</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>" avec le lien "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>follow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>", cela indique aux moteurs de recherche qu'ils doivent indexer la page (index) et suivre les liens présents sur celle-ci (follow)</t>
-    </r>
-  </si>
-  <si>
-    <t>Crawbilité non améliorée pour une meilleur indexation</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ajouter </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&lt;meta name="robots" content="index, follow"&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">dans la balise </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;head&gt;&lt;/head&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>http://robots-txt.com/meta-robots/</t>
-  </si>
-  <si>
-    <r>
-      <t>balise meta "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>keywords</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>" est présente</t>
-    </r>
-  </si>
-  <si>
-    <t>Balise inutile pour le référencement</t>
-  </si>
-  <si>
-    <t>Ne pas mettre cette balise</t>
-  </si>
-  <si>
-    <t>La supprimer du code</t>
-  </si>
-  <si>
-    <t>https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
-  </si>
-  <si>
-    <t>Mauvais pour le référencement, Google est plus à même de comprendre la page si les balises sont claires</t>
-  </si>
-  <si>
-    <t>Toujours utiliser ces balises pour montrer à Google les points importants</t>
-  </si>
-  <si>
-    <t>Les rajouter</t>
-  </si>
-  <si>
-    <t>https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/</t>
-  </si>
-  <si>
-    <r>
-      <t>Manque les balises sémantiques comme "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>header</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>", "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>main</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>", "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>footer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>", etc…</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Balises "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>keywords</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>" inutiles et pratiquant le black hat</t>
-    </r>
-  </si>
-  <si>
-    <t>Ne jamais utiliser cette pratique, toujours insérer les mots-clés de façon naturelle dans du texte ou titres cohérents</t>
-  </si>
-  <si>
-    <t>Supprimer ces balises</t>
-  </si>
-  <si>
-    <t>https://fr.semrush.com/blog/seo-black-hat/</t>
-  </si>
-  <si>
-    <t>Lien sur la page où l'on est, et répétitions de liens vers une même page</t>
-  </si>
-  <si>
-    <t>multiplier les liens vers une même page en variant les ancres est une technique inutile en SEO car elle ne permet pas de positionner notre site sur plusieurs mots-clés.</t>
-  </si>
-  <si>
-    <t>Varier les supports sur lesquels nos liens sont positionnés (exemple image + texte), ou supprimer les liens en trop</t>
-  </si>
-  <si>
-    <t>Supprimer les répétitions des liens</t>
-  </si>
-  <si>
-    <t>https://www.joptimisemonsite.fr/astuce-seo-liens-identiques-meme-page/</t>
-  </si>
-  <si>
-    <t>Très mauvaise pratique de mettre les mots-clés de la même couleur que le fond (invisible pour l'utilisateur mais pas pour Google). Cela pénalise le référencement</t>
-  </si>
-  <si>
-    <t>Images trop lourdes</t>
-  </si>
-  <si>
-    <t>Images sans images mais avec du texte</t>
-  </si>
-  <si>
-    <t>Elles sont inutiles parce que le contenu peut être écrit entre des balises h ou p. Les images servent à illustrer du contenu et alourdissent la page.</t>
-  </si>
-  <si>
-    <t>Supprimer les images de texte et les remplacer par des balises avec du texte à l’intérieur.</t>
-  </si>
-  <si>
-    <t>N’utiliser des images que lorsque c’est nécessaire.</t>
-  </si>
-  <si>
-    <t>https://imageseo.io/images-seo-optimization/</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>alt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>" des images sont des spams, ne décrivent pas l'image</t>
-    </r>
-  </si>
-  <si>
-    <t>Le format des images n’est pas optimisé ce qui ralentit la vitesse du site</t>
-  </si>
-  <si>
-    <t>Favoriser des formats rapide à charger, et toujours dans des dimensions équivalentes à leur div</t>
-  </si>
-  <si>
-    <t>Compresser et changer les images</t>
-  </si>
-  <si>
-    <t>Pas de description de l'image, Google ne va pas comprendre le contenu de nos images + spam</t>
-  </si>
-  <si>
-    <r>
-      <t>Toujours mettre une description de l'image dans l'attribut "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>alt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <t>Mettre une description de l'image</t>
-  </si>
-  <si>
-    <t>Pas assez de contraste sur le bouton "contact" et certains textes par rapport au background</t>
-  </si>
-  <si>
-    <t>Contraste insuffisant et ne permet pas une très bonne visibilité</t>
-  </si>
-  <si>
-    <t>Pour la conformité au niveau AA, le critère de succès WCAG 2.0 1.4.3 recommande que le texte normal ait un rapport de contraste minimum de 4,5:1 et que le texte de grande taille (18 points ou 14 points en gras) ait un rapport de contraste minimum de 3:1</t>
-  </si>
-  <si>
-    <t>Changer la couleur des textes pour avoir un bon ratio de contraste</t>
-  </si>
-  <si>
-    <t>https://dequeuniversity.com/tips/color-contrast</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Balises sémantiques </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> mal structuré</t>
-    </r>
-  </si>
-  <si>
-    <t>Les balises n'ont pas d'ordre hiérarchique</t>
-  </si>
-  <si>
-    <t>Utiliser qu'une seule balise H1, et ensuite les autres balises qui suivent doivent toujours être hierarchisées</t>
-  </si>
-  <si>
-    <t>Changer les hn pour tout hiérarchiser correctement</t>
-  </si>
-  <si>
-    <t>https://rank-it.fr/les-balises-hn/</t>
-  </si>
-  <si>
-    <t>La typographie peut être non visible car trop petite</t>
-  </si>
-  <si>
-    <t>Typographie trop petite</t>
-  </si>
-  <si>
-    <t>Toujours avoir un contenu lisible dès le départ</t>
-  </si>
-  <si>
-    <t>Changer la taille de la police ainsi que le "font-weight" si besoin</t>
-  </si>
-  <si>
-    <t>http://www.pompage.net/traduction/ameliorer-l-accessibilite-par-la-typographie</t>
-  </si>
-  <si>
-    <t>Liens dans le footer</t>
-  </si>
-  <si>
-    <t>Ils n'ont aucun intérêt et aucun rapport avec notre activité</t>
-  </si>
-  <si>
-    <t>Il faut avoir un annuaire dédié ou idéalement mettre les liens relatifs aux contenu dans une balise ancre</t>
-  </si>
-  <si>
-    <t>Supprimer tous les liens du footer</t>
-  </si>
-  <si>
-    <t>https://www.leptidigital.fr/webmarketing/seo/liens-footer-header-sitewide-6974/</t>
-  </si>
-  <si>
-    <t>Mieux espacé les questions et mettre des exemples</t>
-  </si>
-  <si>
-    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6940878-decouvrez-les-exigences-en-matiere-daccessibilite</t>
-  </si>
-  <si>
-    <t>Formulaire pas clair, manque liaison label avec texte</t>
-  </si>
-  <si>
-    <r>
-      <t>Formulaire non espacé et pas d'instructions claires, manque l'attribut "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>for</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>" à "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Fournir de l'aide pour les formulaires + rajouter l'attribut "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>for</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>" ayant la même valeur que l'id du champ</t>
     </r>
   </si>
 </sst>
@@ -1061,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1045"/>
+  <dimension ref="A1:Z1035"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.29296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1119,24 +1113,24 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1145,19 +1139,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1166,19 +1160,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1187,19 +1181,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1208,275 +1202,268 @@
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="F11" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="13" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="16" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="6" t="s">
+    <row r="15" spans="1:26" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="17" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>38</v>
+      <c r="F17" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="18" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="23" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="25" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="27" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="29" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="31" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="10" t="s">
+      <c r="D31" s="8" t="s">
         <v>72</v>
       </c>
+      <c r="E31" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="20" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>43</v>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="33" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="22" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="24" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="28" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="30" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="32" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="37" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="39" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="42" spans="1:6" s="5" customFormat="1" ht="60.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2462,22 +2449,12 @@
     <row r="1033" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="1034" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="1035" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1036" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1037" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1038" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1039" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1040" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1041" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1042" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1043" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1044" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="1045" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F7" r:id="rId3"/>
-    <hyperlink ref="F11" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId2"/>
+    <hyperlink ref="F11" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId5"/>

</xml_diff>